<commit_message>
identifying the wrong comps in parallel drawing functions
</commit_message>
<xml_diff>
--- a/utils/system_history.xlsx
+++ b/utils/system_history.xlsx
@@ -937,16 +937,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -976,19 +976,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1015,19 +1015,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1054,19 +1054,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1093,19 +1093,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1132,19 +1132,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1171,19 +1171,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1210,19 +1210,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>

</xml_diff>

<commit_message>
need to create a better function for creating a list centered on 0
</commit_message>
<xml_diff>
--- a/utils/system_history.xlsx
+++ b/utils/system_history.xlsx
@@ -1054,7 +1054,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1093,7 +1093,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1105,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1132,7 +1132,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1144,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1171,7 +1171,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1210,7 +1210,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>1</v>

</xml_diff>

<commit_message>
staring to draw Systems
</commit_message>
<xml_diff>
--- a/utils/system_history.xlsx
+++ b/utils/system_history.xlsx
@@ -1054,7 +1054,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1093,7 +1093,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1105,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1141,10 +1141,10 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1180,10 +1180,10 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1213,16 +1213,16 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>

</xml_diff>